<commit_message>
SSDM-9544 fix UPDATE_IF_EXISTS mode in xls parser for experiment
</commit_message>
<xml_diff>
--- a/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings.xlsx
+++ b/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/general_eln_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariapukhliakova/git/openbis/openbis_standard_technologies/sourceTest/java/ch/ethz/sis/openbis/systemtest/plugin/excelimport/test_files/samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D90705FB-5ECD-3143-A33F-3BD5A88AD844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDCD605-E3FD-1146-AAE6-E81CD467FB4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{8C518BD6-93EE-234E-BC6F-85CE38D9A7C4}"/>
+    <workbookView xWindow="6360" yWindow="1300" windowWidth="27240" windowHeight="16440" xr2:uid="{8C518BD6-93EE-234E-BC6F-85CE38D9A7C4}"/>
   </bookViews>
   <sheets>
     <sheet name="TYPES" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t>SPACE</t>
   </si>
@@ -104,12 +104,54 @@
   <si>
     <t>$</t>
   </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>EXPERIMENT</t>
+  </si>
+  <si>
+    <t>Experiment type</t>
+  </si>
+  <si>
+    <t>DEFAULT_EXPERIMENT</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Default Experiment</t>
+  </si>
+  <si>
+    <t>/ELN_SETTINGS/DEFAULT_PROJECT</t>
+  </si>
+  <si>
+    <t>DEFAULT_PROJECT</t>
+  </si>
+  <si>
+    <t>Default Project</t>
+  </si>
+  <si>
+    <t>EXPERIMENT_TYPE</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>$NAME</t>
+  </si>
+  <si>
+    <t>General info</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +212,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -191,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -215,6 +273,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,16 +592,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97AFC839-03FA-9149-96B9-6013B98081EB}">
-  <dimension ref="A1:XFC15"/>
+  <dimension ref="A1:XFC31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.5" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="19" x14ac:dyDescent="0.25">
@@ -12937,60 +13002,220 @@
     </row>
     <row r="7" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="D11" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+    <row r="15" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="13"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B27" s="2"/>
     </row>
-    <row r="12" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
     </row>
-    <row r="13" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:1023 1025:2047 2049:3071 3073:4095 4097:5119 5121:6143 6145:7167 7169:8191 8193:9215 9217:10239 10241:11263 11265:12287 12289:13311 13313:14335 14337:15359 15361:16383" x14ac:dyDescent="0.2">
-      <c r="B15" s="2" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>